<commit_message>
Nhà cung cấp nè
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,57 +12,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
-  <si>
-    <t>MaNCC</t>
-  </si>
-  <si>
-    <t>TenNCC</t>
-  </si>
-  <si>
-    <t>SDT</t>
-  </si>
-  <si>
-    <t>DiaChi</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+  <si>
+    <t>Mã nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Tên nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>NCC001</t>
-  </si>
-  <si>
-    <t>DELL</t>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>NCC002</t>
+  </si>
+  <si>
+    <t>ACER</t>
+  </si>
+  <si>
+    <t>0987654321</t>
+  </si>
+  <si>
+    <t>Ð?a ch? ACER</t>
+  </si>
+  <si>
+    <t>acer@example.com</t>
+  </si>
+  <si>
+    <t>NCC003</t>
+  </si>
+  <si>
+    <t>ASUS</t>
   </si>
   <si>
     <t>0123456789</t>
-  </si>
-  <si>
-    <t>Ð?a ch? DELL</t>
-  </si>
-  <si>
-    <t>dell@example.com</t>
-  </si>
-  <si>
-    <t>NCC002</t>
-  </si>
-  <si>
-    <t>ACER</t>
-  </si>
-  <si>
-    <t>0987654321</t>
-  </si>
-  <si>
-    <t>Ð?a ch? ACER</t>
-  </si>
-  <si>
-    <t>acer@example.com</t>
-  </si>
-  <si>
-    <t>NCC003</t>
-  </si>
-  <si>
-    <t>ASUS</t>
   </si>
   <si>
     <t>Ð?a ch? ASUS</t>
@@ -149,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -231,7 +219,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>21</v>
@@ -248,30 +236,13 @@
         <v>24</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>25</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>26</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>